<commit_message>
Inserimento Description_IT e Name_IT
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\Gapminder\d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66B3439F-A122-4FDA-8BA5-FF1E7EE93328}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8C613-ED49-465D-8CB3-A3AC132A7C9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="124">
   <si>
     <t>concept</t>
   </si>
@@ -304,6 +304,108 @@
   </si>
   <si>
     <t>Arbeitslosenquote (AMB-Definition) (Männer)</t>
+  </si>
+  <si>
+    <t>description_DE</t>
+  </si>
+  <si>
+    <t>name_DE</t>
+  </si>
+  <si>
+    <t>name_IT</t>
+  </si>
+  <si>
+    <t>Alto Adige</t>
+  </si>
+  <si>
+    <t>Comuni in Alto Adige</t>
+  </si>
+  <si>
+    <t>Comprensori in Alto Adige</t>
+  </si>
+  <si>
+    <t>Anno di osservazione</t>
+  </si>
+  <si>
+    <t>Quota di stranieri</t>
+  </si>
+  <si>
+    <t>Anno</t>
+  </si>
+  <si>
+    <t>Entrate dei Comuni pro capite</t>
+  </si>
+  <si>
+    <t>Spese dei Comuni pro capite</t>
+  </si>
+  <si>
+    <t>Popolazione</t>
+  </si>
+  <si>
+    <t>Turismo: permanenza media (giorni)</t>
+  </si>
+  <si>
+    <t>Turismo: soggiorni</t>
+  </si>
+  <si>
+    <t>Saldo migratorio</t>
+  </si>
+  <si>
+    <t>Commercio al dettaglio: punti vendita</t>
+  </si>
+  <si>
+    <t>Crescita demografica (‰)</t>
+  </si>
+  <si>
+    <t>Lavoratori dipendenti</t>
+  </si>
+  <si>
+    <t>Lavoratori dipendenti (donne)</t>
+  </si>
+  <si>
+    <t>Lavoratori dipendenti (uomini)</t>
+  </si>
+  <si>
+    <t>Apprendisti</t>
+  </si>
+  <si>
+    <t>Apprendisti (donne)</t>
+  </si>
+  <si>
+    <t>Apprendisti (uomini)</t>
+  </si>
+  <si>
+    <t>Occupati a tempo indeterminato</t>
+  </si>
+  <si>
+    <t>Occupati a tempo indeterminato (donne)</t>
+  </si>
+  <si>
+    <t>Occupati a tempo indeterminato (uomini)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tasso di occupazione dipendente </t>
+  </si>
+  <si>
+    <t>Tasso di occupazione dipendente (donne)</t>
+  </si>
+  <si>
+    <t>Tasso di occupazione dipendente (uomini)</t>
+  </si>
+  <si>
+    <t>Disoccupati iscritti</t>
+  </si>
+  <si>
+    <t>Disoccupati iscritti (donne)</t>
+  </si>
+  <si>
+    <t>Disoccupati iscritti (uomini)</t>
+  </si>
+  <si>
+    <t>Tasso di disoccupazione (OML)= disoccupati iscritti/ (occupati dipendenti + disoccupati iscritti), considerando solo occupati dipendenti residenti e persone di età dai 15 ai 64 anni.</t>
+  </si>
+  <si>
+    <t>description_IT</t>
   </si>
 </sst>
 </file>
@@ -664,20 +766,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="21.5703125" customWidth="1"/>
+    <col min="4" max="4" width="44.5703125" customWidth="1"/>
+    <col min="5" max="5" width="38.28515625" customWidth="1"/>
+    <col min="6" max="7" width="21.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -688,16 +791,22 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -708,10 +817,16 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
+        <v>93</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -725,13 +840,19 @@
         <v>12</v>
       </c>
       <c r="E3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -745,10 +866,16 @@
         <v>16</v>
       </c>
       <c r="E4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -759,10 +886,16 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -773,10 +906,16 @@
         <v>23</v>
       </c>
       <c r="E6" t="s">
+        <v>97</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -787,10 +926,16 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -801,10 +946,16 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -815,10 +966,16 @@
         <v>29</v>
       </c>
       <c r="E9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -829,10 +986,16 @@
         <v>31</v>
       </c>
       <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -843,10 +1006,16 @@
         <v>33</v>
       </c>
       <c r="E11" t="s">
+        <v>103</v>
+      </c>
+      <c r="F11" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -857,10 +1026,16 @@
         <v>35</v>
       </c>
       <c r="E12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>36</v>
       </c>
@@ -871,10 +1046,16 @@
         <v>37</v>
       </c>
       <c r="E13" t="s">
+        <v>105</v>
+      </c>
+      <c r="F13" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>38</v>
       </c>
@@ -885,10 +1066,16 @@
         <v>39</v>
       </c>
       <c r="E14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -896,7 +1083,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -904,7 +1091,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>3</v>
       </c>
@@ -912,7 +1099,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>5</v>
       </c>
@@ -920,7 +1107,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -931,10 +1118,16 @@
         <v>42</v>
       </c>
       <c r="E19" t="s">
+        <v>107</v>
+      </c>
+      <c r="F19" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>44</v>
       </c>
@@ -945,10 +1138,16 @@
         <v>45</v>
       </c>
       <c r="E20" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>47</v>
       </c>
@@ -959,10 +1158,16 @@
         <v>48</v>
       </c>
       <c r="E21" t="s">
+        <v>109</v>
+      </c>
+      <c r="F21" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -973,10 +1178,16 @@
         <v>51</v>
       </c>
       <c r="E22" t="s">
+        <v>110</v>
+      </c>
+      <c r="F22" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>53</v>
       </c>
@@ -987,10 +1198,16 @@
         <v>54</v>
       </c>
       <c r="E23" t="s">
+        <v>111</v>
+      </c>
+      <c r="F23" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -1001,10 +1218,16 @@
         <v>57</v>
       </c>
       <c r="E24" t="s">
+        <v>112</v>
+      </c>
+      <c r="F24" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>59</v>
       </c>
@@ -1015,10 +1238,16 @@
         <v>60</v>
       </c>
       <c r="E25" t="s">
+        <v>113</v>
+      </c>
+      <c r="F25" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>62</v>
       </c>
@@ -1029,10 +1258,16 @@
         <v>63</v>
       </c>
       <c r="E26" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>65</v>
       </c>
@@ -1043,10 +1278,16 @@
         <v>66</v>
       </c>
       <c r="E27" t="s">
+        <v>115</v>
+      </c>
+      <c r="F27" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>68</v>
       </c>
@@ -1057,10 +1298,16 @@
         <v>69</v>
       </c>
       <c r="E28" t="s">
+        <v>116</v>
+      </c>
+      <c r="F28" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
@@ -1071,10 +1318,16 @@
         <v>72</v>
       </c>
       <c r="E29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>74</v>
       </c>
@@ -1085,10 +1338,16 @@
         <v>75</v>
       </c>
       <c r="E30" t="s">
+        <v>118</v>
+      </c>
+      <c r="F30" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1099,10 +1358,16 @@
         <v>78</v>
       </c>
       <c r="E31" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -1113,10 +1378,16 @@
         <v>80</v>
       </c>
       <c r="E32" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>81</v>
       </c>
@@ -1127,10 +1398,16 @@
         <v>82</v>
       </c>
       <c r="E33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F33" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>83</v>
       </c>
@@ -1141,10 +1418,16 @@
         <v>84</v>
       </c>
       <c r="E34" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G34" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1155,10 +1438,16 @@
         <v>84</v>
       </c>
       <c r="E35" t="s">
+        <v>122</v>
+      </c>
+      <c r="F35" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G35" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>88</v>
       </c>
@@ -1169,7 +1458,13 @@
         <v>84</v>
       </c>
       <c r="E36" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" t="s">
         <v>89</v>
+      </c>
+      <c r="G36" t="s">
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
integrated language selection in concepts.xlsx
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB617330-FADD-493A-8EB0-4C5F7E4EA7A4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8C613-ED49-465D-8CB3-A3AC132A7C9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="124">
   <si>
     <t>concept</t>
   </si>
@@ -403,6 +403,9 @@
   </si>
   <si>
     <t>Tasso di disoccupazione (OML)= disoccupati iscritti/ (occupati dipendenti + disoccupati iscritti), considerando solo occupati dipendenti residenti e persone di età dai 15 ai 64 anni.</t>
+  </si>
+  <si>
+    <t>description_IT</t>
   </si>
 </sst>
 </file>
@@ -765,8 +768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
   <dimension ref="A1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:G36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -791,7 +794,7 @@
         <v>90</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>123</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>91</v>

</xml_diff>

<commit_message>
added svg coordinates to xlsx added function to generate geo, comuni and aggregations
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Desktop\PROGETTO\motioncharts\d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMB\ARBDATEN\OnlineGrafiken\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC8C613-ED49-465D-8CB3-A3AC132A7C9D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8D62D9-6D58-440E-83D2-F3A2A1E7574F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="125">
   <si>
     <t>concept</t>
   </si>
@@ -406,6 +403,9 @@
   </si>
   <si>
     <t>description_IT</t>
+  </si>
+  <si>
+    <t>shape_lores_svg</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,7 +470,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -766,13 +766,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="4" max="4" width="44.5703125" customWidth="1"/>
@@ -1467,6 +1467,14 @@
         <v>122</v>
       </c>
     </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>124</v>
+      </c>
+      <c r="B37" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
added tags to xlsx added code to create working ddf file in R
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMB\ARBDATEN\OnlineGrafiken\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E020C636-CD73-4096-A440-CAB422CFAC0D}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CD1C60-BEDE-4790-9465-0C2BA52F4CC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="1770" windowWidth="27405" windowHeight="10230" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="199">
   <si>
     <t>concept</t>
   </si>
@@ -187,9 +187,6 @@
     <t>app</t>
   </si>
   <si>
-    <t>Traditionelle Lehrlinge</t>
-  </si>
-  <si>
     <t>Lehrlinge</t>
   </si>
   <si>
@@ -217,36 +214,24 @@
     <t>Unbefristet Beschäftigte</t>
   </si>
   <si>
-    <t>Unbefr. Beschäftigte</t>
-  </si>
-  <si>
     <t>ind_f</t>
   </si>
   <si>
     <t>Unbefristet Beschäftigte (Frauen)</t>
   </si>
   <si>
-    <t>Unbefr. Besch. (Frauen)</t>
-  </si>
-  <si>
     <t>ind_m</t>
   </si>
   <si>
     <t>Unbefristet Beschäftigte (Männer)</t>
   </si>
   <si>
-    <t>Unbefr. Besch. (Männer)</t>
-  </si>
-  <si>
     <t>tod</t>
   </si>
   <si>
     <t>Unselbständige Beschäftigungsquote</t>
   </si>
   <si>
-    <t>Unselb. Beschäftigungsquote</t>
-  </si>
-  <si>
     <t>tod_f</t>
   </si>
   <si>
@@ -421,9 +406,21 @@
     <t>Beschäftigung</t>
   </si>
   <si>
+    <t>Frauen</t>
+  </si>
+  <si>
+    <t>Männer</t>
+  </si>
+  <si>
+    <t>Insgesamt</t>
+  </si>
+  <si>
     <t>Arbeitslosigkeit</t>
   </si>
   <si>
+    <t>Unbefristet</t>
+  </si>
+  <si>
     <t>Tags</t>
   </si>
   <si>
@@ -442,18 +439,6 @@
     <t>Color</t>
   </si>
   <si>
-    <t>Life expectancy, female</t>
-  </si>
-  <si>
-    <t>Life expectancy, male</t>
-  </si>
-  <si>
-    <t>Number of child deaths</t>
-  </si>
-  <si>
-    <t>Underweight children</t>
-  </si>
-  <si>
     <t>tag</t>
   </si>
   <si>
@@ -502,14 +487,155 @@
     <t>Tag</t>
   </si>
   <si>
-    <t>occupazione_apprendisti</t>
+    <t>indeterminato</t>
+  </si>
+  <si>
+    <t>Indeterminato</t>
+  </si>
+  <si>
+    <t>Traditionelle Lehrlinge (Insgesamt)</t>
+  </si>
+  <si>
+    <t>Apprendisti (totale)</t>
+  </si>
+  <si>
+    <t>Lehrlinge (Insgesamt)</t>
+  </si>
+  <si>
+    <t>Totale</t>
+  </si>
+  <si>
+    <t>Donne</t>
+  </si>
+  <si>
+    <t>Uomini</t>
+  </si>
+  <si>
+    <t>dipendente</t>
+  </si>
+  <si>
+    <t>Unselb. Beschäftigte</t>
+  </si>
+  <si>
+    <t>Occupazione dipendente</t>
+  </si>
+  <si>
+    <t>name_catalog_DE</t>
+  </si>
+  <si>
+    <t>name_short_DE</t>
+  </si>
+  <si>
+    <t>name_catalog_IT</t>
+  </si>
+  <si>
+    <t>name_short_IT</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote (Insgesamt)</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote (Frauen)</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote (Männer)</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote, Insgesamt</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote, Männer</t>
+  </si>
+  <si>
+    <t>Arbeitslosenquote, Frauen</t>
+  </si>
+  <si>
+    <t>astat</t>
+  </si>
+  <si>
+    <t>Gemeindeindikatoren</t>
+  </si>
+  <si>
+    <t>Indicatori comunali</t>
+  </si>
+  <si>
+    <t>Arbeitslose (Insgesamt)</t>
+  </si>
+  <si>
+    <t>Registrierte Arbeitslose (Insgesamt)</t>
+  </si>
+  <si>
+    <t>Registrierte Arbeitslose (Frauen)</t>
+  </si>
+  <si>
+    <t>Registrierte Arbeitslose (Männer)</t>
+  </si>
+  <si>
+    <t>Arbeitslose (Frauen)</t>
+  </si>
+  <si>
+    <t>Arbeitslose (Männer)</t>
+  </si>
+  <si>
+    <t>Unselb. Beschäftigungsquote (Insgesamt)</t>
+  </si>
+  <si>
+    <t>_root, astat</t>
+  </si>
+  <si>
+    <t>scales</t>
+  </si>
+  <si>
+    <t>source</t>
+  </si>
+  <si>
+    <t>source_long</t>
+  </si>
+  <si>
+    <t>source_url</t>
+  </si>
+  <si>
+    <t>["linear", "log"]</t>
+  </si>
+  <si>
+    <t>https://qlikview.services.siag.it/QvAJAXZfc/opendoc_notool.htm?document=gemeindedatenblatt.qvw&amp;host=QVS%40titan-a&amp;anonymous=true</t>
+  </si>
+  <si>
+    <t>source_DE</t>
+  </si>
+  <si>
+    <t>source_IT</t>
+  </si>
+  <si>
+    <t>ASTAT (amtliche Wohnbevölkerung)</t>
+  </si>
+  <si>
+    <t>Source URL</t>
+  </si>
+  <si>
+    <t>Source Long Text</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Scales</t>
+  </si>
+  <si>
+    <t>Amtliche Wohnbevölkerung</t>
+  </si>
+  <si>
+    <t>Popolazione ufficiale</t>
+  </si>
+  <si>
+    <t>ASTAT (popolazione ufficiale)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -521,6 +647,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,14 +677,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -863,31 +1000,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" customWidth="1"/>
-    <col min="6" max="6" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="34.28515625" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
     <col min="7" max="7" width="17.5703125" customWidth="1"/>
     <col min="8" max="8" width="24.85546875" customWidth="1"/>
-    <col min="10" max="10" width="23.28515625" customWidth="1"/>
-    <col min="11" max="11" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="23.28515625" customWidth="1"/>
+    <col min="12" max="13" width="15.140625" customWidth="1"/>
+    <col min="14" max="14" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="13" customWidth="1"/>
+    <col min="17" max="17" width="24.140625" customWidth="1"/>
+    <col min="18" max="18" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -896,118 +1037,139 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>125</v>
+        <v>162</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>126</v>
+        <v>164</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2" t="s">
+        <v>117</v>
+      </c>
+      <c r="G2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J2" t="s">
+        <v>169</v>
+      </c>
+      <c r="L2" t="s">
+        <v>166</v>
+      </c>
+      <c r="S2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H3" t="s">
+        <v>117</v>
+      </c>
+      <c r="J3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L3" t="s">
+        <v>167</v>
+      </c>
+      <c r="S3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>83</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
         <v>84</v>
       </c>
-      <c r="F2" t="s">
-        <v>122</v>
-      </c>
-      <c r="G2" t="s">
-        <v>85</v>
-      </c>
-      <c r="H2" t="s">
-        <v>122</v>
-      </c>
-      <c r="J2" t="s">
-        <v>136</v>
-      </c>
-      <c r="K2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G3" t="s">
-        <v>87</v>
-      </c>
-      <c r="H3" t="s">
-        <v>122</v>
-      </c>
-      <c r="J3" t="s">
-        <v>137</v>
-      </c>
-      <c r="K3" t="s">
-        <v>137</v>
-      </c>
-      <c r="L3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" t="s">
-        <v>122</v>
-      </c>
-      <c r="G4" t="s">
-        <v>89</v>
-      </c>
       <c r="H4" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="J4" t="s">
-        <v>138</v>
-      </c>
-      <c r="K4" t="s">
-        <v>138</v>
+        <v>170</v>
       </c>
       <c r="L4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+      <c r="S4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -1015,74 +1177,77 @@
         <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>153</v>
       </c>
       <c r="F5" t="s">
-        <v>110</v>
+        <v>154</v>
       </c>
       <c r="G5" t="s">
+        <v>126</v>
+      </c>
+      <c r="H5" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" t="s">
+        <v>155</v>
+      </c>
+      <c r="S5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>52</v>
       </c>
-      <c r="H5" t="s">
-        <v>110</v>
-      </c>
-      <c r="J5" t="s">
-        <v>139</v>
-      </c>
-      <c r="K5" t="s">
-        <v>139</v>
-      </c>
-      <c r="L5" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
         <v>53</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" t="s">
+        <v>157</v>
+      </c>
+      <c r="L6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="S6" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>56</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
+        <v>107</v>
+      </c>
+      <c r="G7" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" t="s">
+        <v>158</v>
+      </c>
+      <c r="L7" t="s">
         <v>57</v>
       </c>
-      <c r="F7" t="s">
-        <v>112</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="s">
-        <v>112</v>
-      </c>
-      <c r="L7" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -1096,132 +1261,150 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G8" t="s">
         <v>17</v>
       </c>
       <c r="H8" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
         <v>40</v>
       </c>
       <c r="G9" t="s">
-        <v>135</v>
-      </c>
-      <c r="L9" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="S9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>3</v>
       </c>
       <c r="C10" t="s">
         <v>40</v>
       </c>
-      <c r="L10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S10" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" t="s">
+        <v>114</v>
+      </c>
+      <c r="G11" t="s">
+        <v>126</v>
+      </c>
+      <c r="H11" t="s">
+        <v>156</v>
+      </c>
+      <c r="J11" t="s">
+        <v>175</v>
+      </c>
+      <c r="L11" t="s">
+        <v>176</v>
+      </c>
+      <c r="S11" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" t="s">
+        <v>115</v>
+      </c>
+      <c r="G12" t="s">
+        <v>124</v>
+      </c>
+      <c r="H12" t="s">
+        <v>157</v>
+      </c>
+      <c r="J12" t="s">
+        <v>179</v>
+      </c>
+      <c r="L12" t="s">
+        <v>177</v>
+      </c>
+      <c r="S12" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" t="s">
         <v>77</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>78</v>
-      </c>
-      <c r="F11" t="s">
-        <v>119</v>
-      </c>
-      <c r="G11" t="s">
-        <v>78</v>
-      </c>
-      <c r="H11" t="s">
-        <v>119</v>
-      </c>
-      <c r="L11" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>79</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>80</v>
-      </c>
-      <c r="F12" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12" t="s">
-        <v>80</v>
-      </c>
-      <c r="H12" t="s">
-        <v>120</v>
-      </c>
-      <c r="L12" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>81</v>
-      </c>
-      <c r="C13" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" t="s">
-        <v>82</v>
-      </c>
       <c r="F13" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="G13" t="s">
-        <v>82</v>
+        <v>125</v>
       </c>
       <c r="H13" t="s">
-        <v>121</v>
+        <v>158</v>
+      </c>
+      <c r="J13" t="s">
+        <v>180</v>
       </c>
       <c r="L13" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="S13" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>2</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="L14" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S14" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
       </c>
-      <c r="L15" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -1232,16 +1415,19 @@
         <v>25</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="G16" t="s">
         <v>25</v>
       </c>
       <c r="H16" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+      <c r="S16" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -1255,19 +1441,19 @@
         <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="G17" t="s">
         <v>13</v>
       </c>
       <c r="H17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I17" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1278,16 +1464,16 @@
         <v>8</v>
       </c>
       <c r="F18" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G18" t="s">
         <v>9</v>
       </c>
       <c r="H18" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>28</v>
       </c>
@@ -1298,88 +1484,94 @@
         <v>29</v>
       </c>
       <c r="F19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="G19" t="s">
         <v>29</v>
       </c>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="J19" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>29</v>
+      </c>
+      <c r="S19" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
-        <v>22</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" t="s">
+        <v>156</v>
+      </c>
+      <c r="S20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>60</v>
       </c>
-      <c r="F20" t="s">
-        <v>113</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" t="s">
         <v>61</v>
       </c>
-      <c r="H20" t="s">
-        <v>113</v>
-      </c>
-      <c r="L20" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F21" t="s">
+        <v>109</v>
+      </c>
+      <c r="G21" t="s">
+        <v>124</v>
+      </c>
+      <c r="H21" t="s">
+        <v>157</v>
+      </c>
+      <c r="S21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>62</v>
       </c>
-      <c r="C21" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" t="s">
+      <c r="C22" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" t="s">
         <v>63</v>
       </c>
-      <c r="F21" t="s">
-        <v>114</v>
-      </c>
-      <c r="G21" t="s">
-        <v>64</v>
-      </c>
-      <c r="H21" t="s">
-        <v>114</v>
-      </c>
-      <c r="L21" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>65</v>
-      </c>
-      <c r="C22" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" t="s">
-        <v>66</v>
-      </c>
       <c r="F22" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="H22" t="s">
-        <v>115</v>
-      </c>
-      <c r="L22" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+      <c r="S22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>34</v>
       </c>
@@ -1390,16 +1582,19 @@
         <v>35</v>
       </c>
       <c r="F23" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G23" t="s">
         <v>35</v>
       </c>
       <c r="H23" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+      <c r="S23" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>4</v>
       </c>
@@ -1407,41 +1602,41 @@
         <v>40</v>
       </c>
       <c r="G24" t="s">
-        <v>154</v>
-      </c>
-      <c r="L24" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="S24" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C25" t="s">
         <v>40</v>
       </c>
       <c r="G25" t="s">
-        <v>132</v>
-      </c>
-      <c r="L25" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S25" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C26" t="s">
         <v>40</v>
       </c>
       <c r="G26" t="s">
-        <v>133</v>
-      </c>
-      <c r="L26" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+        <v>132</v>
+      </c>
+      <c r="S26" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -1452,19 +1647,22 @@
         <v>42</v>
       </c>
       <c r="F27" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="G27" t="s">
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="L27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+        <v>126</v>
+      </c>
+      <c r="S27" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -1475,19 +1673,22 @@
         <v>45</v>
       </c>
       <c r="F28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G28" t="s">
         <v>46</v>
       </c>
       <c r="H28" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="L28" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+        <v>124</v>
+      </c>
+      <c r="S28" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>47</v>
       </c>
@@ -1498,33 +1699,36 @@
         <v>48</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="G29" t="s">
         <v>49</v>
       </c>
       <c r="H29" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L29" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="S29" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C30" t="s">
         <v>40</v>
       </c>
       <c r="G30" t="s">
-        <v>153</v>
-      </c>
-      <c r="L30" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+      <c r="S30" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
@@ -1535,16 +1739,22 @@
         <v>23</v>
       </c>
       <c r="F31" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G31" t="s">
         <v>23</v>
       </c>
       <c r="H31" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+      <c r="L31" t="s">
+        <v>23</v>
+      </c>
+      <c r="S31" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1552,19 +1762,37 @@
         <v>22</v>
       </c>
       <c r="E32" t="s">
-        <v>31</v>
+        <v>196</v>
       </c>
       <c r="F32" t="s">
-        <v>101</v>
+        <v>197</v>
       </c>
       <c r="G32" t="s">
         <v>31</v>
       </c>
       <c r="H32" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="L32" t="s">
+        <v>31</v>
+      </c>
+      <c r="N32" t="s">
+        <v>187</v>
+      </c>
+      <c r="O32" t="s">
+        <v>191</v>
+      </c>
+      <c r="P32" t="s">
+        <v>198</v>
+      </c>
+      <c r="R32" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="S32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1575,16 +1803,22 @@
         <v>39</v>
       </c>
       <c r="F33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="G33" t="s">
         <v>39</v>
       </c>
       <c r="H33" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="L33" t="s">
+        <v>39</v>
+      </c>
+      <c r="S33" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1595,19 +1829,25 @@
         <v>33</v>
       </c>
       <c r="F34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="G34" t="s">
         <v>33</v>
       </c>
       <c r="H34" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="J34" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L34" t="s">
+        <v>33</v>
+      </c>
+      <c r="S34" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1618,27 +1858,33 @@
         <v>37</v>
       </c>
       <c r="F35" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
       </c>
       <c r="H35" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="L35" t="s">
+        <v>37</v>
+      </c>
+      <c r="S35" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
         <v>40</v>
       </c>
-      <c r="L36" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="S36" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>26</v>
       </c>
@@ -1649,44 +1895,47 @@
         <v>27</v>
       </c>
       <c r="F37" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G37" t="s">
         <v>27</v>
       </c>
       <c r="H37" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+      <c r="S37" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C38" t="s">
         <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
-      </c>
-      <c r="L38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+      <c r="S38" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C39" t="s">
         <v>40</v>
       </c>
       <c r="G39" t="s">
+        <v>129</v>
+      </c>
+      <c r="S39" t="s">
         <v>130</v>
       </c>
-      <c r="L39" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>18</v>
       </c>
@@ -1697,174 +1946,286 @@
         <v>19</v>
       </c>
       <c r="F40" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="G40" t="s">
         <v>20</v>
       </c>
       <c r="H40" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C41" t="s">
+        <v>22</v>
+      </c>
+      <c r="E41" t="s">
+        <v>65</v>
+      </c>
+      <c r="F41" t="s">
+        <v>111</v>
+      </c>
+      <c r="G41" t="s">
+        <v>126</v>
+      </c>
+      <c r="H41" t="s">
+        <v>156</v>
+      </c>
+      <c r="L41" t="s">
+        <v>181</v>
+      </c>
+      <c r="S41" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>66</v>
+      </c>
+      <c r="C42" t="s">
+        <v>22</v>
+      </c>
+      <c r="E42" t="s">
+        <v>67</v>
+      </c>
+      <c r="F42" t="s">
+        <v>112</v>
+      </c>
+      <c r="G42" t="s">
+        <v>124</v>
+      </c>
+      <c r="H42" t="s">
+        <v>157</v>
+      </c>
+      <c r="L42" t="s">
         <v>68</v>
       </c>
-      <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="S42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>69</v>
       </c>
-      <c r="F41" t="s">
-        <v>116</v>
-      </c>
-      <c r="G41" t="s">
+      <c r="C43" t="s">
+        <v>22</v>
+      </c>
+      <c r="E43" t="s">
         <v>70</v>
       </c>
-      <c r="H41" t="s">
-        <v>116</v>
-      </c>
-      <c r="L41" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="F43" t="s">
+        <v>113</v>
+      </c>
+      <c r="G43" t="s">
+        <v>125</v>
+      </c>
+      <c r="H43" t="s">
+        <v>158</v>
+      </c>
+      <c r="L43" t="s">
         <v>71</v>
       </c>
-      <c r="C42" t="s">
-        <v>22</v>
-      </c>
-      <c r="E42" t="s">
-        <v>72</v>
-      </c>
-      <c r="F42" t="s">
-        <v>117</v>
-      </c>
-      <c r="G42" t="s">
-        <v>73</v>
-      </c>
-      <c r="H42" t="s">
-        <v>117</v>
-      </c>
-      <c r="L42" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>74</v>
-      </c>
-      <c r="C43" t="s">
-        <v>22</v>
-      </c>
-      <c r="E43" t="s">
-        <v>75</v>
-      </c>
-      <c r="F43" t="s">
-        <v>118</v>
-      </c>
-      <c r="G43" t="s">
-        <v>76</v>
-      </c>
-      <c r="H43" t="s">
-        <v>118</v>
-      </c>
-      <c r="L43" t="s">
-        <v>145</v>
+      <c r="S43" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>186</v>
+      </c>
+      <c r="C44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G44" t="s">
+        <v>192</v>
+      </c>
+      <c r="S44" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>185</v>
+      </c>
+      <c r="C45" t="s">
+        <v>40</v>
+      </c>
+      <c r="G45" t="s">
+        <v>193</v>
+      </c>
+      <c r="S45" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>184</v>
+      </c>
+      <c r="C46" t="s">
+        <v>40</v>
+      </c>
+      <c r="G46" t="s">
+        <v>194</v>
+      </c>
+      <c r="S46" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>183</v>
+      </c>
+      <c r="C47" t="s">
+        <v>40</v>
+      </c>
+      <c r="G47" t="s">
+        <v>195</v>
+      </c>
+      <c r="S47" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L43">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M43">
     <sortCondition ref="A2:A43"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="R32" r:id="rId1" xr:uid="{4E63C2E5-16AB-4DB2-834A-C416D957E989}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85885AD-D562-4BAD-8623-0E641ACFDAAD}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" t="s">
-        <v>92</v>
-      </c>
-      <c r="D1" t="s">
-        <v>141</v>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+      <c r="C3" t="s">
         <v>145</v>
-      </c>
-      <c r="B3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C3" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="D6" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>151</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>152</v>
+      </c>
+      <c r="D7" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>159</v>
+      </c>
+      <c r="B8" t="s">
+        <v>160</v>
+      </c>
+      <c r="C8" t="s">
+        <v>161</v>
+      </c>
+      <c r="D8" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+      <c r="C9" t="s">
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed substring of GEM for municipalities and added last year as copy of previous year at ASTAT data
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMB\ARBDATEN\OnlineGrafiken\motioncharts\d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNiedermair\Documents\Motioncharts\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2CD1C60-BEDE-4790-9465-0C2BA52F4CC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8803C3D-9138-4C19-B460-201AE6B3B3E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="207">
   <si>
     <t>concept</t>
   </si>
@@ -629,6 +629,30 @@
   </si>
   <si>
     <t>ASTAT (popolazione ufficiale)</t>
+  </si>
+  <si>
+    <t>Tasso di disoccupazione (donne)</t>
+  </si>
+  <si>
+    <t>Tasso di disoccupazione (totale)</t>
+  </si>
+  <si>
+    <t>Tasso di disoccupazione (uomini)</t>
+  </si>
+  <si>
+    <t>Disoccupati iscritti (totale)</t>
+  </si>
+  <si>
+    <t>Turismo: permanenza media (gg)</t>
+  </si>
+  <si>
+    <t>Occupati tempo indeterminato (totale)</t>
+  </si>
+  <si>
+    <t>Occupati tempo indeterminato (donne)</t>
+  </si>
+  <si>
+    <t>Occupati tempo indeterminato (uomini)</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
   <dimension ref="A1:S47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P33" sqref="P33"/>
+    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
+      <selection activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,6 +1131,9 @@
       <c r="L2" t="s">
         <v>166</v>
       </c>
+      <c r="M2" t="s">
+        <v>200</v>
+      </c>
       <c r="S2" t="s">
         <v>141</v>
       </c>
@@ -1136,6 +1163,9 @@
       <c r="L3" t="s">
         <v>167</v>
       </c>
+      <c r="M3" t="s">
+        <v>199</v>
+      </c>
       <c r="S3" t="s">
         <v>141</v>
       </c>
@@ -1165,6 +1195,9 @@
       <c r="L4" t="s">
         <v>168</v>
       </c>
+      <c r="M4" t="s">
+        <v>201</v>
+      </c>
       <c r="S4" t="s">
         <v>141</v>
       </c>
@@ -1191,6 +1224,9 @@
       <c r="L5" t="s">
         <v>155</v>
       </c>
+      <c r="M5" t="s">
+        <v>154</v>
+      </c>
       <c r="S5" t="s">
         <v>142</v>
       </c>
@@ -1217,6 +1253,9 @@
       <c r="L6" t="s">
         <v>54</v>
       </c>
+      <c r="M6" t="s">
+        <v>106</v>
+      </c>
       <c r="S6" t="s">
         <v>142</v>
       </c>
@@ -1243,6 +1282,9 @@
       <c r="L7" t="s">
         <v>57</v>
       </c>
+      <c r="M7" t="s">
+        <v>107</v>
+      </c>
       <c r="S7" t="s">
         <v>142</v>
       </c>
@@ -1320,6 +1362,9 @@
       <c r="L11" t="s">
         <v>176</v>
       </c>
+      <c r="M11" t="s">
+        <v>202</v>
+      </c>
       <c r="S11" t="s">
         <v>138</v>
       </c>
@@ -1349,6 +1394,9 @@
       <c r="L12" t="s">
         <v>177</v>
       </c>
+      <c r="M12" t="s">
+        <v>115</v>
+      </c>
       <c r="S12" t="s">
         <v>138</v>
       </c>
@@ -1378,6 +1426,9 @@
       <c r="L13" t="s">
         <v>178</v>
       </c>
+      <c r="M13" t="s">
+        <v>116</v>
+      </c>
       <c r="S13" t="s">
         <v>138</v>
       </c>
@@ -1498,6 +1549,9 @@
       <c r="L19" t="s">
         <v>29</v>
       </c>
+      <c r="M19" t="s">
+        <v>203</v>
+      </c>
       <c r="S19" t="s">
         <v>172</v>
       </c>
@@ -1521,6 +1575,9 @@
       <c r="H20" t="s">
         <v>156</v>
       </c>
+      <c r="M20" t="s">
+        <v>204</v>
+      </c>
       <c r="S20" t="s">
         <v>151</v>
       </c>
@@ -1544,6 +1601,9 @@
       <c r="H21" t="s">
         <v>157</v>
       </c>
+      <c r="M21" t="s">
+        <v>205</v>
+      </c>
       <c r="S21" t="s">
         <v>151</v>
       </c>
@@ -1567,6 +1627,9 @@
       <c r="H22" t="s">
         <v>158</v>
       </c>
+      <c r="M22" t="s">
+        <v>206</v>
+      </c>
       <c r="S22" t="s">
         <v>151</v>
       </c>
@@ -1588,6 +1651,9 @@
         <v>35</v>
       </c>
       <c r="H23" t="s">
+        <v>99</v>
+      </c>
+      <c r="M23" t="s">
         <v>99</v>
       </c>
       <c r="S23" t="s">

</xml_diff>

<commit_message>
merge con local file
</commit_message>
<xml_diff>
--- a/d/concepts.xlsx
+++ b/d/concepts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WNiedermair\Documents\Motioncharts\motioncharts\d\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\AMB\ARBDATEN\OnlineGrafiken\motioncharts\d\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8803C3D-9138-4C19-B460-201AE6B3B3E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{301D9F1A-674A-45F7-A452-1F3A98344DB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{06B255CA-2E7D-4A4E-9BF4-FBB011BE254E}"/>
   </bookViews>
   <sheets>
     <sheet name="concept" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="210">
   <si>
     <t>concept</t>
   </si>
@@ -76,12 +76,6 @@
     <t>Gemeinde</t>
   </si>
   <si>
-    <t>["bez"]</t>
-  </si>
-  <si>
-    <t>bez</t>
-  </si>
-  <si>
     <t>Bezirke in Südtirol</t>
   </si>
   <si>
@@ -631,28 +625,43 @@
     <t>ASTAT (popolazione ufficiale)</t>
   </si>
   <si>
-    <t>Tasso di disoccupazione (donne)</t>
-  </si>
-  <si>
-    <t>Tasso di disoccupazione (totale)</t>
-  </si>
-  <si>
-    <t>Tasso di disoccupazione (uomini)</t>
-  </si>
-  <si>
-    <t>Disoccupati iscritti (totale)</t>
-  </si>
-  <si>
-    <t>Turismo: permanenza media (gg)</t>
-  </si>
-  <si>
-    <t>Occupati tempo indeterminato (totale)</t>
-  </si>
-  <si>
-    <t>Occupati tempo indeterminato (donne)</t>
-  </si>
-  <si>
-    <t>Occupati tempo indeterminato (uomini)</t>
+    <t>asdimora</t>
+  </si>
+  <si>
+    <t>pafdimora</t>
+  </si>
+  <si>
+    <t>dimora</t>
+  </si>
+  <si>
+    <t>Funktionale Kleinregionen</t>
+  </si>
+  <si>
+    <t>Piccole Aree Funzionali</t>
+  </si>
+  <si>
+    <t>FKR</t>
+  </si>
+  <si>
+    <t>PAF</t>
+  </si>
+  <si>
+    <t>Ges. Bezirke in Südtirol</t>
+  </si>
+  <si>
+    <t>Circoscrizioni</t>
+  </si>
+  <si>
+    <t>Ges. Bezirke</t>
+  </si>
+  <si>
+    <t>["asdimora","dimora"]</t>
+  </si>
+  <si>
+    <t>categorizations</t>
+  </si>
+  <si>
+    <t>Categorizations</t>
   </si>
 </sst>
 </file>
@@ -1024,10 +1033,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{534EF0F7-B23F-4FF4-8AC3-187B801533BE}">
-  <dimension ref="A1:S47"/>
+  <dimension ref="A1:S49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E19" workbookViewId="0">
-      <selection activeCell="M27" sqref="M27"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1052,7 +1061,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -1061,237 +1070,219 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>87</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="L1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="N1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>185</v>
-      </c>
       <c r="R1" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" t="s">
         <v>78</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" t="s">
-        <v>79</v>
-      </c>
-      <c r="F2" t="s">
-        <v>117</v>
-      </c>
-      <c r="G2" t="s">
-        <v>80</v>
-      </c>
       <c r="H2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L2" t="s">
-        <v>166</v>
-      </c>
-      <c r="M2" t="s">
-        <v>200</v>
+        <v>164</v>
       </c>
       <c r="S2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L3" t="s">
-        <v>167</v>
-      </c>
-      <c r="M3" t="s">
-        <v>199</v>
+        <v>165</v>
       </c>
       <c r="S3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="J4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="L4" t="s">
-        <v>168</v>
-      </c>
-      <c r="M4" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="S4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="s">
+        <v>151</v>
+      </c>
+      <c r="F5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H5" t="s">
+        <v>154</v>
+      </c>
+      <c r="L5" t="s">
         <v>153</v>
       </c>
-      <c r="F5" t="s">
-        <v>154</v>
-      </c>
-      <c r="G5" t="s">
-        <v>126</v>
-      </c>
-      <c r="H5" t="s">
-        <v>156</v>
-      </c>
-      <c r="L5" t="s">
-        <v>155</v>
-      </c>
-      <c r="M5" t="s">
-        <v>154</v>
-      </c>
       <c r="S5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" t="s">
+        <v>104</v>
+      </c>
+      <c r="G6" t="s">
+        <v>122</v>
+      </c>
+      <c r="H6" t="s">
+        <v>155</v>
+      </c>
+      <c r="L6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" t="s">
-        <v>106</v>
-      </c>
-      <c r="G6" t="s">
-        <v>124</v>
-      </c>
-      <c r="H6" t="s">
-        <v>157</v>
-      </c>
-      <c r="L6" t="s">
-        <v>54</v>
-      </c>
-      <c r="M6" t="s">
-        <v>106</v>
-      </c>
       <c r="S6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>54</v>
+      </c>
+      <c r="F7" t="s">
+        <v>105</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7" t="s">
+        <v>156</v>
+      </c>
+      <c r="L7" t="s">
         <v>55</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" t="s">
-        <v>56</v>
-      </c>
-      <c r="F7" t="s">
-        <v>107</v>
-      </c>
-      <c r="G7" t="s">
-        <v>125</v>
-      </c>
-      <c r="H7" t="s">
-        <v>158</v>
-      </c>
-      <c r="L7" t="s">
-        <v>57</v>
-      </c>
-      <c r="M7" t="s">
-        <v>107</v>
-      </c>
       <c r="S7" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>197</v>
       </c>
       <c r="C8" t="s">
         <v>11</v>
@@ -1300,617 +1291,596 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>16</v>
+        <v>204</v>
       </c>
       <c r="F8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>206</v>
       </c>
       <c r="H8" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="S8" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>133</v>
+        <v>198</v>
       </c>
       <c r="C9" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F9" t="s">
+        <v>201</v>
       </c>
       <c r="G9" t="s">
-        <v>134</v>
+        <v>202</v>
+      </c>
+      <c r="H9" t="s">
+        <v>203</v>
       </c>
       <c r="S9" t="s">
-        <v>130</v>
+        <v>208</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>199</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" t="s">
+        <v>88</v>
+      </c>
+      <c r="G10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" t="s">
+        <v>205</v>
       </c>
       <c r="S10" t="s">
-        <v>130</v>
+        <v>208</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>131</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" t="s">
-        <v>73</v>
-      </c>
-      <c r="F11" t="s">
-        <v>114</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>126</v>
-      </c>
-      <c r="H11" t="s">
-        <v>156</v>
-      </c>
-      <c r="J11" t="s">
-        <v>175</v>
-      </c>
-      <c r="L11" t="s">
-        <v>176</v>
-      </c>
-      <c r="M11" t="s">
-        <v>202</v>
+        <v>132</v>
       </c>
       <c r="S11" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="F12" t="s">
-        <v>115</v>
-      </c>
-      <c r="G12" t="s">
-        <v>124</v>
-      </c>
-      <c r="H12" t="s">
-        <v>157</v>
-      </c>
-      <c r="J12" t="s">
-        <v>179</v>
-      </c>
-      <c r="L12" t="s">
-        <v>177</v>
-      </c>
-      <c r="M12" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="S12" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="F13" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="J13" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="L13" t="s">
-        <v>178</v>
-      </c>
-      <c r="M13" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="S13" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>72</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" t="s">
+        <v>113</v>
+      </c>
+      <c r="G14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H14" t="s">
+        <v>155</v>
+      </c>
+      <c r="J14" t="s">
+        <v>177</v>
+      </c>
+      <c r="L14" t="s">
+        <v>175</v>
       </c>
       <c r="S14" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>74</v>
       </c>
       <c r="C15" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+      <c r="F15" t="s">
+        <v>114</v>
+      </c>
+      <c r="G15" t="s">
+        <v>123</v>
+      </c>
+      <c r="H15" t="s">
+        <v>156</v>
+      </c>
+      <c r="J15" t="s">
+        <v>178</v>
+      </c>
+      <c r="L15" t="s">
+        <v>176</v>
       </c>
       <c r="S15" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" t="s">
-        <v>94</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="S16" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I17" t="s">
-        <v>14</v>
+        <v>38</v>
+      </c>
+      <c r="S17" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E18" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F18" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>88</v>
+        <v>92</v>
+      </c>
+      <c r="S18" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="G19" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="H19" t="s">
-        <v>97</v>
-      </c>
-      <c r="J19" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" t="s">
-        <v>203</v>
+        <v>87</v>
+      </c>
+      <c r="I19" t="s">
+        <v>207</v>
       </c>
       <c r="S19" t="s">
-        <v>172</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E20" t="s">
-        <v>59</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="G20" t="s">
-        <v>126</v>
+        <v>9</v>
       </c>
       <c r="H20" t="s">
-        <v>156</v>
-      </c>
-      <c r="M20" t="s">
-        <v>204</v>
-      </c>
-      <c r="S20" t="s">
-        <v>151</v>
+        <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>60</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>61</v>
+        <v>27</v>
       </c>
       <c r="F21" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="G21" t="s">
-        <v>124</v>
+        <v>27</v>
       </c>
       <c r="H21" t="s">
-        <v>157</v>
-      </c>
-      <c r="M21" t="s">
-        <v>205</v>
+        <v>95</v>
+      </c>
+      <c r="J21" t="s">
+        <v>27</v>
+      </c>
+      <c r="L21" t="s">
+        <v>27</v>
       </c>
       <c r="S21" t="s">
-        <v>151</v>
+        <v>170</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E22" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F22" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G22" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H22" t="s">
-        <v>158</v>
-      </c>
-      <c r="M22" t="s">
-        <v>206</v>
+        <v>154</v>
       </c>
       <c r="S22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>58</v>
       </c>
       <c r="C23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" t="s">
-        <v>35</v>
+        <v>59</v>
       </c>
       <c r="F23" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="G23" t="s">
-        <v>35</v>
+        <v>122</v>
       </c>
       <c r="H23" t="s">
-        <v>99</v>
-      </c>
-      <c r="M23" t="s">
-        <v>99</v>
+        <v>155</v>
       </c>
       <c r="S23" t="s">
-        <v>172</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="C24" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24" t="s">
+        <v>108</v>
       </c>
       <c r="G24" t="s">
+        <v>123</v>
+      </c>
+      <c r="H24" t="s">
+        <v>156</v>
+      </c>
+      <c r="S24" t="s">
         <v>149</v>
-      </c>
-      <c r="S24" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>120</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25" t="s">
+        <v>97</v>
       </c>
       <c r="G25" t="s">
-        <v>131</v>
+        <v>33</v>
+      </c>
+      <c r="H25" t="s">
+        <v>97</v>
       </c>
       <c r="S25" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>121</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G26" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="S26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>41</v>
+        <v>118</v>
       </c>
       <c r="C27" t="s">
-        <v>22</v>
-      </c>
-      <c r="E27" t="s">
-        <v>42</v>
-      </c>
-      <c r="F27" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="G27" t="s">
-        <v>43</v>
-      </c>
-      <c r="H27" t="s">
-        <v>102</v>
-      </c>
-      <c r="L27" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="S27" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>119</v>
       </c>
       <c r="C28" t="s">
-        <v>22</v>
-      </c>
-      <c r="E28" t="s">
-        <v>45</v>
-      </c>
-      <c r="F28" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="G28" t="s">
-        <v>46</v>
-      </c>
-      <c r="H28" t="s">
-        <v>103</v>
-      </c>
-      <c r="L28" t="s">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="S28" t="s">
-        <v>159</v>
+        <v>128</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C29" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E29" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="F29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G29" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="H29" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L29" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S29" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>136</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E30" t="s">
+        <v>43</v>
+      </c>
+      <c r="F30" t="s">
+        <v>101</v>
       </c>
       <c r="G30" t="s">
-        <v>148</v>
+        <v>44</v>
+      </c>
+      <c r="H30" t="s">
+        <v>101</v>
+      </c>
+      <c r="L30" t="s">
+        <v>122</v>
       </c>
       <c r="S30" t="s">
-        <v>130</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E31" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="F31" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="L31" t="s">
-        <v>23</v>
+        <v>123</v>
       </c>
       <c r="S31" t="s">
-        <v>172</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>134</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
-      </c>
-      <c r="E32" t="s">
-        <v>196</v>
-      </c>
-      <c r="F32" t="s">
-        <v>197</v>
+        <v>38</v>
       </c>
       <c r="G32" t="s">
-        <v>31</v>
-      </c>
-      <c r="H32" t="s">
-        <v>96</v>
-      </c>
-      <c r="L32" t="s">
-        <v>31</v>
-      </c>
-      <c r="N32" t="s">
-        <v>187</v>
-      </c>
-      <c r="O32" t="s">
-        <v>191</v>
-      </c>
-      <c r="P32" t="s">
-        <v>198</v>
-      </c>
-      <c r="R32" s="2" t="s">
-        <v>188</v>
+        <v>146</v>
       </c>
       <c r="S32" t="s">
-        <v>182</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="F33" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G33" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="H33" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="L33" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="S33" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E34" t="s">
-        <v>33</v>
+        <v>194</v>
       </c>
       <c r="F34" t="s">
-        <v>98</v>
+        <v>195</v>
       </c>
       <c r="G34" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H34" t="s">
-        <v>98</v>
-      </c>
-      <c r="J34" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
       <c r="L34" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="N34" t="s">
+        <v>185</v>
+      </c>
+      <c r="O34" t="s">
+        <v>189</v>
+      </c>
+      <c r="P34" t="s">
+        <v>196</v>
+      </c>
+      <c r="R34" s="2" t="s">
+        <v>186</v>
       </c>
       <c r="S34" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
@@ -1918,213 +1888,240 @@
         <v>36</v>
       </c>
       <c r="C35" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E35" t="s">
         <v>37</v>
       </c>
       <c r="F35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G35" t="s">
         <v>37</v>
       </c>
       <c r="H35" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="L35" t="s">
         <v>37</v>
       </c>
       <c r="S35" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>119</v>
+        <v>30</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E36" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" t="s">
+        <v>96</v>
+      </c>
+      <c r="J36" t="s">
+        <v>31</v>
+      </c>
+      <c r="L36" t="s">
+        <v>31</v>
       </c>
       <c r="S36" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C37" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E37" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F37" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G37" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="H37" t="s">
-        <v>95</v>
+        <v>98</v>
+      </c>
+      <c r="L37" t="s">
+        <v>35</v>
       </c>
       <c r="S37" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>150</v>
+        <v>38</v>
       </c>
       <c r="S38" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>122</v>
+        <v>24</v>
       </c>
       <c r="C39" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E39" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" t="s">
+        <v>93</v>
       </c>
       <c r="G39" t="s">
-        <v>129</v>
+        <v>25</v>
+      </c>
+      <c r="H39" t="s">
+        <v>93</v>
       </c>
       <c r="S39" t="s">
-        <v>130</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>18</v>
+        <v>133</v>
       </c>
       <c r="C40" t="s">
-        <v>18</v>
-      </c>
-      <c r="E40" t="s">
-        <v>19</v>
-      </c>
-      <c r="F40" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>20</v>
-      </c>
-      <c r="H40" t="s">
-        <v>93</v>
+        <v>148</v>
+      </c>
+      <c r="S40" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>64</v>
+        <v>120</v>
       </c>
       <c r="C41" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" t="s">
-        <v>65</v>
-      </c>
-      <c r="F41" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="G41" t="s">
-        <v>126</v>
-      </c>
-      <c r="H41" t="s">
-        <v>156</v>
-      </c>
-      <c r="L41" t="s">
-        <v>181</v>
+        <v>127</v>
       </c>
       <c r="S41" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="C42" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E42" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
       <c r="F42" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="G42" t="s">
-        <v>124</v>
+        <v>18</v>
       </c>
       <c r="H42" t="s">
-        <v>157</v>
-      </c>
-      <c r="L42" t="s">
-        <v>68</v>
-      </c>
-      <c r="S42" t="s">
-        <v>140</v>
+        <v>91</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E43" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="F43" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="G43" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="H43" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="L43" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
       <c r="S43" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>64</v>
       </c>
       <c r="C44" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E44" t="s">
+        <v>65</v>
+      </c>
+      <c r="F44" t="s">
+        <v>110</v>
       </c>
       <c r="G44" t="s">
-        <v>192</v>
+        <v>122</v>
+      </c>
+      <c r="H44" t="s">
+        <v>155</v>
+      </c>
+      <c r="L44" t="s">
+        <v>66</v>
       </c>
       <c r="S44" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>185</v>
+        <v>67</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>20</v>
+      </c>
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+      <c r="F45" t="s">
+        <v>111</v>
       </c>
       <c r="G45" t="s">
-        <v>193</v>
+        <v>123</v>
+      </c>
+      <c r="H45" t="s">
+        <v>156</v>
+      </c>
+      <c r="L45" t="s">
+        <v>69</v>
       </c>
       <c r="S45" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
@@ -2132,13 +2129,13 @@
         <v>184</v>
       </c>
       <c r="C46" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G46" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="S46" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
@@ -2146,21 +2143,49 @@
         <v>183</v>
       </c>
       <c r="C47" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G47" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="S47" t="s">
-        <v>130</v>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>182</v>
+      </c>
+      <c r="C48" t="s">
+        <v>38</v>
+      </c>
+      <c r="G48" t="s">
+        <v>192</v>
+      </c>
+      <c r="S48" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>181</v>
+      </c>
+      <c r="C49" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" t="s">
+        <v>193</v>
+      </c>
+      <c r="S49" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M43">
-    <sortCondition ref="A2:A43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M45">
+    <sortCondition ref="A2:A45"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="R32" r:id="rId1" xr:uid="{4E63C2E5-16AB-4DB2-834A-C416D957E989}"/>
+    <hyperlink ref="R34" r:id="rId1" xr:uid="{4E63C2E5-16AB-4DB2-834A-C416D957E989}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
@@ -2169,10 +2194,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C85885AD-D562-4BAD-8623-0E641ACFDAAD}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2185,113 +2210,124 @@
   <sheetData>
     <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B3" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" t="s">
         <v>143</v>
-      </c>
-      <c r="C3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>157</v>
+      </c>
+      <c r="B8" t="s">
+        <v>158</v>
+      </c>
+      <c r="C8" t="s">
         <v>159</v>
       </c>
-      <c r="B8" t="s">
-        <v>160</v>
-      </c>
-      <c r="C8" t="s">
-        <v>161</v>
-      </c>
       <c r="D8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" t="s">
         <v>172</v>
       </c>
-      <c r="B9" t="s">
-        <v>173</v>
-      </c>
-      <c r="C9" t="s">
-        <v>174</v>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>208</v>
+      </c>
+      <c r="B10" t="s">
+        <v>209</v>
+      </c>
+      <c r="C10" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>